<commit_message>
update basefile.xlsx as example
</commit_message>
<xml_diff>
--- a/testing/data_test/basefile.xlsx
+++ b/testing/data_test/basefile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altz7\PycharmProjects\ENBIOS4TIMES_\testing\data_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB88BC9B-4A22-4A05-BF00-A1ADAFC7A0A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11316CCF-D5F9-4066-B7C6-519BD9FFFB93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{DEDD0F12-97D4-4533-B747-9AB0A3FFB504}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="89">
   <si>
     <t>wind_onshore</t>
   </si>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t>81174ec2c20931c1a36f65c654bbd11e</t>
-  </si>
-  <si>
-    <t>46839adbc3cf15621ddbbe687eaa6df1</t>
   </si>
   <si>
     <t>b870e3d3ddd5b634d016940064b27532</t>
@@ -296,10 +293,16 @@
     <t>Ecoinvent_key_code</t>
   </si>
   <si>
-    <t>ssss</t>
+    <t>06412182</t>
   </si>
   <si>
-    <t>06412182</t>
+    <t>File_source</t>
+  </si>
+  <si>
+    <t>nameplate_capacity.csv</t>
+  </si>
+  <si>
+    <t>flow_out_sum.csv</t>
   </si>
 </sst>
 </file>
@@ -617,6 +620,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -627,9 +633,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -948,8 +951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3C39739-7903-4A57-97A6-9EAA12556E85}">
   <dimension ref="A1:I776"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B23" zoomScale="113" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -961,12 +964,12 @@
     <col min="6" max="6" width="25.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="22.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>16</v>
@@ -978,9 +981,11 @@
         <v>18</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
-      <c r="G1" s="6"/>
+      <c r="G1" s="6" t="s">
+        <v>86</v>
+      </c>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
     </row>
@@ -989,7 +994,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -1003,16 +1008,18 @@
       <c r="F2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="6"/>
+      <c r="G2" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1</v>
@@ -1024,10 +1031,10 @@
         <v>1000000000</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>86</v>
+        <v>22</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>23</v>
+      <c r="G3" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -1037,7 +1044,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>1</v>
@@ -1049,9 +1056,11 @@
         <v>1000000000</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="G4" s="6"/>
+      <c r="G4" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
     </row>
@@ -1060,7 +1069,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>1</v>
@@ -1072,9 +1081,11 @@
         <v>1000000000</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
-      <c r="G5" s="6"/>
+      <c r="G5" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
     </row>
@@ -1083,7 +1094,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>1</v>
@@ -1095,9 +1106,11 @@
         <v>1000000000</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
-      <c r="G6" s="6"/>
+      <c r="G6" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
     </row>
@@ -1106,7 +1119,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>1</v>
@@ -1118,9 +1131,11 @@
         <v>1000000000</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
-      <c r="G7" s="6"/>
+      <c r="G7" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
     </row>
@@ -1129,7 +1144,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>1</v>
@@ -1141,18 +1156,20 @@
         <v>1000000000</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
-      <c r="G8" s="6"/>
+      <c r="G8" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>1</v>
@@ -1164,9 +1181,11 @@
         <v>1000000000</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
-      <c r="G9" s="6"/>
+      <c r="G9" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
     </row>
@@ -1175,7 +1194,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>1</v>
@@ -1189,7 +1208,9 @@
       <c r="F10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="6"/>
+      <c r="G10" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
@@ -1198,7 +1219,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>1</v>
@@ -1210,9 +1231,11 @@
         <v>1000000000</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
-      <c r="G11" s="6"/>
+      <c r="G11" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
@@ -1221,7 +1244,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>1</v>
@@ -1233,9 +1256,11 @@
         <v>1000000000</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
-      <c r="G12" s="6"/>
+      <c r="G12" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
     </row>
@@ -1244,7 +1269,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>1</v>
@@ -1256,9 +1281,11 @@
         <v>1000000000</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
-      <c r="G13" s="6"/>
+      <c r="G13" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
     </row>
@@ -1267,7 +1294,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>1</v>
@@ -1279,9 +1306,11 @@
         <v>1000000000</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
-      <c r="G14" s="6"/>
+      <c r="G14" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
     </row>
@@ -1290,10 +1319,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>2</v>
@@ -1302,9 +1331,11 @@
         <v>1000000000</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
-      <c r="G15" s="6"/>
+      <c r="G15" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
     </row>
@@ -1313,44 +1344,48 @@
         <v>7</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E16" s="10">
         <v>3600000000</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
-      <c r="G16" s="6"/>
+      <c r="G16" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
     </row>
     <row r="17" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E17" s="10">
         <v>3600000000</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
-      <c r="G17" s="26"/>
+      <c r="G17" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="H17" s="26"/>
       <c r="I17" s="26"/>
     </row>
@@ -1359,21 +1394,23 @@
         <v>12</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E18" s="10">
         <v>3600000000</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
-      <c r="G18" s="9"/>
+      <c r="G18" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
     </row>
@@ -1382,322 +1419,350 @@
         <v>13</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E19" s="10">
         <v>3600000000</v>
       </c>
       <c r="F19" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+    </row>
+    <row r="20" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-    </row>
-    <row r="20" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="9" t="s">
-        <v>36</v>
-      </c>
       <c r="B20" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E20" s="10">
         <v>3600000000</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
-      <c r="G20" s="6"/>
+      <c r="G20" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
     </row>
     <row r="21" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E21" s="10">
         <v>3600000000</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
-      <c r="G21" s="6"/>
+      <c r="G21" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
     </row>
     <row r="22" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E22" s="13">
         <f>60490000</f>
         <v>60490000</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
-      <c r="G22" s="6"/>
+      <c r="G22" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
     </row>
     <row r="23" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E23" s="13">
         <v>2630</v>
       </c>
       <c r="F23" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+    </row>
+    <row r="24" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-    </row>
-    <row r="24" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="12" t="s">
-        <v>42</v>
-      </c>
       <c r="B24" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E24" s="13">
         <v>5230</v>
       </c>
       <c r="F24" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+    </row>
+    <row r="25" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-    </row>
-    <row r="25" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="12" t="s">
-        <v>62</v>
+      <c r="D25" s="12" t="s">
+        <v>39</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>77</v>
+      <c r="E25" s="13" t="s">
+        <v>80</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="F25" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="12" t="s">
-        <v>40</v>
+      <c r="G25" s="6" t="s">
+        <v>88</v>
       </c>
-      <c r="E25" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="F25" s="12" t="s">
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+    </row>
+    <row r="26" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-    </row>
-    <row r="26" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="12" t="s">
-        <v>46</v>
-      </c>
       <c r="B26" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E26" s="13">
         <v>1000000000</v>
       </c>
       <c r="F26" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+    </row>
+    <row r="27" spans="1:9" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-    </row>
-    <row r="27" spans="1:9" ht="22.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="14" t="s">
-        <v>48</v>
-      </c>
       <c r="B27" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C27" s="14" t="s">
         <v>1</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E27" s="15">
         <v>1000000000</v>
       </c>
       <c r="F27" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+    </row>
+    <row r="28" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
-    </row>
-    <row r="28" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="17" t="s">
+      <c r="B28" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C28" s="17" t="s">
+      <c r="D28" s="17" t="s">
         <v>52</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>53</v>
       </c>
       <c r="E28" s="18">
         <v>133000000</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
-      <c r="G28" s="19"/>
+      <c r="G28" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="H28" s="19"/>
       <c r="I28" s="19"/>
     </row>
     <row r="29" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E29" s="18">
         <v>133000000</v>
       </c>
       <c r="F29" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+    </row>
+    <row r="30" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-    </row>
-    <row r="30" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="17" t="s">
-        <v>55</v>
-      </c>
       <c r="B30" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E30" s="18">
         <v>23600000</v>
       </c>
       <c r="F30" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+    </row>
+    <row r="31" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-    </row>
-    <row r="31" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="17" t="s">
+      <c r="B31" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>58</v>
-      </c>
       <c r="D31" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E31" s="18">
         <v>159000000</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
-      <c r="G31" s="19"/>
+      <c r="G31" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="H31" s="19"/>
       <c r="I31" s="19"/>
     </row>
-    <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E32" s="20">
         <f>30084235</f>
         <v>30084235</v>
       </c>
-      <c r="F32" s="31" t="s">
-        <v>87</v>
+      <c r="F32" s="27" t="s">
+        <v>85</v>
       </c>
-      <c r="G32" s="6"/>
+      <c r="G32" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
     </row>
@@ -9807,10 +9872,10 @@
     </row>
     <row r="2" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="29"/>
       <c r="D2" s="4"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
@@ -9841,8 +9906,8 @@
       <c r="A3" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="29"/>
       <c r="D3" s="4"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -9871,10 +9936,10 @@
     </row>
     <row r="4" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="28"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="29"/>
       <c r="D4" s="4"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
@@ -9903,10 +9968,10 @@
     </row>
     <row r="5" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="28"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="29"/>
       <c r="D5" s="4"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
@@ -9935,10 +10000,10 @@
     </row>
     <row r="6" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="28"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="29"/>
       <c r="D6" s="4"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -9966,8 +10031,8 @@
       <c r="AB6" s="6"/>
     </row>
     <row r="7" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="27"/>
-      <c r="C7" s="28"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="29"/>
       <c r="D7" s="4"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -9995,8 +10060,8 @@
       <c r="AB7" s="6"/>
     </row>
     <row r="8" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="27"/>
-      <c r="C8" s="28"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="29"/>
       <c r="D8" s="4"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -10024,8 +10089,8 @@
       <c r="AB8" s="6"/>
     </row>
     <row r="9" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="27"/>
-      <c r="C9" s="28"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="29"/>
       <c r="D9" s="4"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -10053,8 +10118,8 @@
       <c r="AB9" s="6"/>
     </row>
     <row r="10" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="27"/>
-      <c r="C10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="29"/>
       <c r="D10" s="4"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -10082,8 +10147,8 @@
       <c r="AB10" s="6"/>
     </row>
     <row r="11" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="27"/>
-      <c r="C11" s="28"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="29"/>
       <c r="D11" s="4"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
@@ -10111,8 +10176,8 @@
       <c r="AB11" s="6"/>
     </row>
     <row r="12" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="27"/>
-      <c r="C12" s="28"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="29"/>
       <c r="D12" s="4"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
@@ -10140,8 +10205,8 @@
       <c r="AB12" s="6"/>
     </row>
     <row r="13" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="27"/>
-      <c r="C13" s="28"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="29"/>
       <c r="D13" s="4"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
@@ -10170,8 +10235,8 @@
     </row>
     <row r="14" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="28"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="29"/>
       <c r="D14" s="4"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -10200,8 +10265,8 @@
     </row>
     <row r="15" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="28"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="29"/>
       <c r="D15" s="4"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -10230,8 +10295,8 @@
     </row>
     <row r="16" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="28"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="29"/>
       <c r="D16" s="4"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -10260,8 +10325,8 @@
     </row>
     <row r="17" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="28"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="29"/>
       <c r="D17" s="4"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
@@ -10290,8 +10355,8 @@
     </row>
     <row r="18" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="28"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="29"/>
       <c r="D18" s="4"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
@@ -10320,8 +10385,8 @@
     </row>
     <row r="19" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="28"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="29"/>
       <c r="D19" s="4"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
@@ -10350,10 +10415,10 @@
     </row>
     <row r="20" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="30"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="31"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
@@ -10380,10 +10445,10 @@
     </row>
     <row r="21" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4"/>
-      <c r="B21" s="29"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="30"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="31"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
@@ -10410,10 +10475,10 @@
     </row>
     <row r="22" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="30"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="31"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
@@ -10440,10 +10505,10 @@
     </row>
     <row r="23" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="30"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="31"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
@@ -40350,55 +40415,55 @@
     </row>
     <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="22" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="21" t="s">
+    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="21" t="s">
-        <v>69</v>
-      </c>
       <c r="B4" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -40406,65 +40471,65 @@
         <v>2</v>
       </c>
       <c r="B7" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>66</v>
+      <c r="C9" s="12" t="s">
+        <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="11" t="s">
-        <v>32</v>
+    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="11" t="s">
+        <v>39</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B10" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>69</v>
-      </c>
       <c r="C10" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>